<commit_message>
add TC 15, 16
</commit_message>
<xml_diff>
--- a/document/tcs (5).xlsx
+++ b/document/tcs (5).xlsx
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92:C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>